<commit_message>
All panels return correct result range
</commit_message>
<xml_diff>
--- a/ExcelReportGenerator.Tests/TestData/DataSourceDynamicPanelDataSetRenderTest/TestDynamicPanelAfterRenderEvent.xlsx
+++ b/ExcelReportGenerator.Tests/TestData/DataSourceDynamicPanelDataSetRenderTest/TestDynamicPanelAfterRenderEvent.xlsx
@@ -106,7 +106,7 @@
     <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="165" fontId="0" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
@@ -119,7 +119,7 @@
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -428,19 +428,19 @@
       <x:c r="B2" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="C2" s="0" t="s">
+      <x:c r="C2" s="1" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
+      <x:c r="D2" s="1" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="E2" s="0" t="s">
+      <x:c r="E2" s="1" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="F2" s="0" t="s">
+      <x:c r="F2" s="1" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="G2" s="0" t="s">
+      <x:c r="G2" s="1" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
@@ -448,12 +448,14 @@
       <x:c r="B3" s="1" t="n">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C3" s="0" t="s">
+      <x:c r="C3" s="1" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="D3" s="0" t="b">
+      <x:c r="D3" s="1" t="b">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="E3" s="1" t="s"/>
+      <x:c r="F3" s="1" t="s"/>
       <x:c r="G3" s="2" t="n">
         <x:v>523635.93</x:v>
       </x:c>
@@ -462,16 +464,16 @@
       <x:c r="B4" s="1" t="n">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="C4" s="0" t="s">
+      <x:c r="C4" s="1" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D4" s="0" t="b">
+      <x:c r="D4" s="1" t="b">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="E4" s="0" t="n">
+      <x:c r="E4" s="1" t="n">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="F4" s="0" t="s">
+      <x:c r="F4" s="1" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="G4" s="2" t="s"/>
@@ -480,10 +482,12 @@
       <x:c r="B5" s="1" t="n">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="C5" s="0" t="s">
+      <x:c r="C5" s="1" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="F5" s="0" t="s">
+      <x:c r="D5" s="1" t="s"/>
+      <x:c r="E5" s="1" t="s"/>
+      <x:c r="F5" s="1" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="G5" s="2" t="n">
@@ -492,6 +496,10 @@
     </x:row>
     <x:row r="6" spans="1:17">
       <x:c r="B6" s="1" t="s"/>
+      <x:c r="C6" s="1" t="s"/>
+      <x:c r="D6" s="1" t="s"/>
+      <x:c r="E6" s="1" t="s"/>
+      <x:c r="F6" s="1" t="s"/>
       <x:c r="G6" s="2" t="n">
         <x:v>623636.4832</x:v>
       </x:c>

</xml_diff>